<commit_message>
make sure all functions work and saving new data can be called from combine_event_data.R
</commit_message>
<xml_diff>
--- a/data/unique_aff.xlsx
+++ b/data/unique_aff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nlesc.sharepoint.com/sites/community/Shared Documents/data_analysis_events/NLeSc_workshop_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{122AC586-BCAB-4246-8B9C-3E336DC4A906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{793D71C8-1555-1544-A706-6EEDB64FBF2A}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{122AC586-BCAB-4246-8B9C-3E336DC4A906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8B2942-7299-244E-9765-65333D39F9A6}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15020" xr2:uid="{5305868D-7B4F-4A49-978B-E34432471178}"/>
   </bookViews>
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F45B2B4-7534-CB46-A4BA-39D7578F3E45}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="C270" sqref="C270"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="A250" sqref="A250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2884,7 +2884,7 @@
         <v>92</v>
       </c>
       <c r="C86" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D86" t="s">
         <v>10</v>
@@ -2901,7 +2901,7 @@
         <v>92</v>
       </c>
       <c r="C87" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -2918,7 +2918,7 @@
         <v>92</v>
       </c>
       <c r="C88" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -6370,6 +6370,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F329B473B817EF4BAF5EC941AA9636D2" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60154e84d3bc079b0db6bb959eaaa164">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e79fd3a6-737d-4cf1-803d-364f639fed05" xmlns:ns3="3c1663fb-7c6c-47a6-a0f9-4709fb897591" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c12652e51acc1204cefa138f9d55f75" ns2:_="" ns3:_="">
     <xsd:import namespace="e79fd3a6-737d-4cf1-803d-364f639fed05"/>
@@ -6580,22 +6595,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE4D51F-0054-48D0-83AF-D1DF8CDDAD88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4B0F45-4307-4958-BD31-77C29ECE3F28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3c1663fb-7c6c-47a6-a0f9-4709fb897591"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e79fd3a6-737d-4cf1-803d-364f639fed05"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DCFD315-7CA8-4537-8120-109CE1150E9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6612,29 +6637,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4B0F45-4307-4958-BD31-77C29ECE3F28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3c1663fb-7c6c-47a6-a0f9-4709fb897591"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e79fd3a6-737d-4cf1-803d-364f639fed05"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE4D51F-0054-48D0-83AF-D1DF8CDDAD88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>